<commit_message>
Draw circle location on the map
</commit_message>
<xml_diff>
--- a/public/files/Danhsach.xlsx
+++ b/public/files/Danhsach.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
   <si>
     <t>STT</t>
   </si>
@@ -918,6 +918,12 @@
   </si>
   <si>
     <t>1979 – 1981, 1983, 1986 – 1987, 1993 - 2002</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Lat</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1047,6 +1053,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1328,21 +1340,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1358,8 +1370,14 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1375,8 +1393,16 @@
       <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <f>104+(((18*60)+(0))/3600)</f>
+        <v>104.3</v>
+      </c>
+      <c r="H2">
+        <f>21+(((3*60)+(0))/3600)</f>
+        <v>21.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1392,8 +1418,16 @@
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <f>104+(((25*60)+(0))/3600)</f>
+        <v>104.41666666666667</v>
+      </c>
+      <c r="H3">
+        <f>21+(((15*60)+(0))/3600)</f>
+        <v>21.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1409,8 +1443,16 @@
       <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <f>104+(((9*60)+(0))/3600)</f>
+        <v>104.15</v>
+      </c>
+      <c r="H4">
+        <f>21+(((36*60)+(12))/3600)</f>
+        <v>21.603333333333332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1426,8 +1468,16 @@
       <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <f>104+(((30*60)+(50))/3600)</f>
+        <v>104.51388888888889</v>
+      </c>
+      <c r="H5">
+        <f>21+(((52*60)+(20))/3600)</f>
+        <v>21.872222222222224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1443,8 +1493,16 @@
       <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <f>104+(((21*60)+(28))/3600)</f>
+        <v>104.35777777777778</v>
+      </c>
+      <c r="H6">
+        <f>21+(((12*60)+(28))/3600)</f>
+        <v>21.207777777777778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1457,7 +1515,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1473,8 +1531,16 @@
       <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <f>103+(((29*60)+(0))/3600)</f>
+        <v>103.48333333333333</v>
+      </c>
+      <c r="H8">
+        <f>22+(((25*60)+(0))/3600)</f>
+        <v>22.416666666666668</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1490,8 +1556,16 @@
       <c r="E9" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <f>103+(((14*60)+(0))/3600)</f>
+        <v>103.23333333333333</v>
+      </c>
+      <c r="H9">
+        <f>22+(((22*60)+(0))/3600)</f>
+        <v>22.366666666666667</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1504,7 +1578,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1520,8 +1594,16 @@
       <c r="E11" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <f>104+(((42*60)+(0))/3600)</f>
+        <v>104.7</v>
+      </c>
+      <c r="H11">
+        <f>20+(((51*60)+(0))/3600)</f>
+        <v>20.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1537,8 +1619,16 @@
       <c r="E12" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <f>104+(((54*60)+(0))/3600)</f>
+        <v>104.9</v>
+      </c>
+      <c r="H12">
+        <f>20+(((20*60)+(0))/3600)</f>
+        <v>20.333333333333332</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1554,8 +1644,16 @@
       <c r="E13" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <f>104+(((44*60)+(0))/3600)</f>
+        <v>104.73333333333333</v>
+      </c>
+      <c r="H13">
+        <f>21+(((4*60)+(0))/3600)</f>
+        <v>21.066666666666666</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1571,8 +1669,16 @@
       <c r="E14" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <f>104+(((9*60)+(0))/3600)</f>
+        <v>104.15</v>
+      </c>
+      <c r="H14">
+        <f>21+(((8*60)+(0))/3600)</f>
+        <v>21.133333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1588,8 +1694,16 @@
       <c r="E15" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <f>104+(((38*60)+(0))/3600)</f>
+        <v>104.63333333333334</v>
+      </c>
+      <c r="H15">
+        <f>21+(((16*60)+(0))/3600)</f>
+        <v>21.266666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1605,8 +1719,16 @@
       <c r="E16" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f>104+(((44*60)+(0))/3600)</f>
+        <v>104.73333333333333</v>
+      </c>
+      <c r="H16">
+        <f>21+(((8*60)+(0))/3600)</f>
+        <v>21.133333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="7" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1622,8 +1744,16 @@
       <c r="E17" s="4" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="7">
+        <f>104+(((46*60)+(50))/3600)</f>
+        <v>104.78055555555555</v>
+      </c>
+      <c r="H17" s="7">
+        <f>20+(((50*60)+(30))/3600)</f>
+        <v>20.841666666666665</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1639,8 +1769,16 @@
       <c r="E18" s="5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="7">
+        <f>104+(((49*60)+(0))/3600)</f>
+        <v>104.81666666666666</v>
+      </c>
+      <c r="H18" s="7">
+        <f>20+(((48*60)+(0))/3600)</f>
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1656,8 +1794,16 @@
       <c r="E19" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="7">
+        <f>103+(((9*60)+(0))/3600)</f>
+        <v>103.15</v>
+      </c>
+      <c r="H19" s="7">
+        <f>22+(((4*60)+(0))/3600)</f>
+        <v>22.066666666666666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1672,6 +1818,14 @@
       </c>
       <c r="E20" s="4" t="s">
         <v>72</v>
+      </c>
+      <c r="G20" s="7">
+        <f>105+(((4*60)+(0))/3600)</f>
+        <v>105.06666666666666</v>
+      </c>
+      <c r="H20" s="7">
+        <f>20+(((46*60)+(0))/3600)</f>
+        <v>20.766666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix "List Station" table
</commit_message>
<xml_diff>
--- a/public/files/Danhsach.xlsx
+++ b/public/files/Danhsach.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>STT</t>
   </si>
@@ -918,12 +918,6 @@
   </si>
   <si>
     <t>1979 – 1981, 1983, 1986 – 1987, 1993 - 2002</t>
-  </si>
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Lat</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1031,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1052,9 +1046,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1340,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,7 +1345,7 @@
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1370,14 +1361,8 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1393,16 +1378,8 @@
       <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G2">
-        <f>104+(((18*60)+(0))/3600)</f>
-        <v>104.3</v>
-      </c>
-      <c r="H2">
-        <f>21+(((3*60)+(0))/3600)</f>
-        <v>21.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1418,16 +1395,8 @@
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G3">
-        <f>104+(((25*60)+(0))/3600)</f>
-        <v>104.41666666666667</v>
-      </c>
-      <c r="H3">
-        <f>21+(((15*60)+(0))/3600)</f>
-        <v>21.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1443,16 +1412,8 @@
       <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G4">
-        <f>104+(((9*60)+(0))/3600)</f>
-        <v>104.15</v>
-      </c>
-      <c r="H4">
-        <f>21+(((36*60)+(12))/3600)</f>
-        <v>21.603333333333332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1468,16 +1429,8 @@
       <c r="E5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G5">
-        <f>104+(((30*60)+(50))/3600)</f>
-        <v>104.51388888888889</v>
-      </c>
-      <c r="H5">
-        <f>21+(((52*60)+(20))/3600)</f>
-        <v>21.872222222222224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1493,16 +1446,8 @@
       <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G6">
-        <f>104+(((21*60)+(28))/3600)</f>
-        <v>104.35777777777778</v>
-      </c>
-      <c r="H6">
-        <f>21+(((12*60)+(28))/3600)</f>
-        <v>21.207777777777778</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:5" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1515,7 +1460,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1531,16 +1476,8 @@
       <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G8">
-        <f>103+(((29*60)+(0))/3600)</f>
-        <v>103.48333333333333</v>
-      </c>
-      <c r="H8">
-        <f>22+(((25*60)+(0))/3600)</f>
-        <v>22.416666666666668</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1556,16 +1493,8 @@
       <c r="E9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G9">
-        <f>103+(((14*60)+(0))/3600)</f>
-        <v>103.23333333333333</v>
-      </c>
-      <c r="H9">
-        <f>22+(((22*60)+(0))/3600)</f>
-        <v>22.366666666666667</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1578,7 +1507,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1594,16 +1523,8 @@
       <c r="E11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G11">
-        <f>104+(((42*60)+(0))/3600)</f>
-        <v>104.7</v>
-      </c>
-      <c r="H11">
-        <f>20+(((51*60)+(0))/3600)</f>
-        <v>20.85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1619,16 +1540,8 @@
       <c r="E12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G12">
-        <f>104+(((54*60)+(0))/3600)</f>
-        <v>104.9</v>
-      </c>
-      <c r="H12">
-        <f>20+(((20*60)+(0))/3600)</f>
-        <v>20.333333333333332</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1644,16 +1557,8 @@
       <c r="E13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G13">
-        <f>104+(((44*60)+(0))/3600)</f>
-        <v>104.73333333333333</v>
-      </c>
-      <c r="H13">
-        <f>21+(((4*60)+(0))/3600)</f>
-        <v>21.066666666666666</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1669,16 +1574,8 @@
       <c r="E14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G14">
-        <f>104+(((9*60)+(0))/3600)</f>
-        <v>104.15</v>
-      </c>
-      <c r="H14">
-        <f>21+(((8*60)+(0))/3600)</f>
-        <v>21.133333333333333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1694,16 +1591,8 @@
       <c r="E15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G15">
-        <f>104+(((38*60)+(0))/3600)</f>
-        <v>104.63333333333334</v>
-      </c>
-      <c r="H15">
-        <f>21+(((16*60)+(0))/3600)</f>
-        <v>21.266666666666666</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1719,16 +1608,8 @@
       <c r="E16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G16">
-        <f>104+(((44*60)+(0))/3600)</f>
-        <v>104.73333333333333</v>
-      </c>
-      <c r="H16">
-        <f>21+(((8*60)+(0))/3600)</f>
-        <v>21.133333333333333</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="7" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" s="6" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1744,16 +1625,8 @@
       <c r="E17" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="7">
-        <f>104+(((46*60)+(50))/3600)</f>
-        <v>104.78055555555555</v>
-      </c>
-      <c r="H17" s="7">
-        <f>20+(((50*60)+(30))/3600)</f>
-        <v>20.841666666666665</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1769,16 +1642,8 @@
       <c r="E18" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="7">
-        <f>104+(((49*60)+(0))/3600)</f>
-        <v>104.81666666666666</v>
-      </c>
-      <c r="H18" s="7">
-        <f>20+(((48*60)+(0))/3600)</f>
-        <v>20.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1794,16 +1659,8 @@
       <c r="E19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="7">
-        <f>103+(((9*60)+(0))/3600)</f>
-        <v>103.15</v>
-      </c>
-      <c r="H19" s="7">
-        <f>22+(((4*60)+(0))/3600)</f>
-        <v>22.066666666666666</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1818,14 +1675,6 @@
       </c>
       <c r="E20" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="G20" s="7">
-        <f>105+(((4*60)+(0))/3600)</f>
-        <v>105.06666666666666</v>
-      </c>
-      <c r="H20" s="7">
-        <f>20+(((46*60)+(0))/3600)</f>
-        <v>20.766666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>